<commit_message>
just for recording: full refactor whole parts of codes.
</commit_message>
<xml_diff>
--- a/meta/program/BlancoRestGeneratorConstants.xlsx
+++ b/meta/program/BlancoRestGeneratorConstants.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoRestGenerator/meta/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B9B41C6-1ACE-F944-B73C-55AA28BBD29C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41A4EADB-58DB-5344-9CCD-5FA326823284}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7100" yWindow="620" windowWidth="21680" windowHeight="11060" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1460" yWindow="1700" windowWidth="22700" windowHeight="15280" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="constants" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="153">
   <si>
     <t>定数定義書</t>
   </si>
@@ -310,10 +310,6 @@
     <phoneticPr fontId="4"/>
   </si>
   <si>
-    <t>"blanco.rest.common.ApiBase"</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
     <t>"getGetRequestId"</t>
     <phoneticPr fontId="4"/>
   </si>
@@ -416,10 +412,6 @@
     <phoneticPr fontId="4"/>
   </si>
   <si>
-    <t>"blanco.rest.Exception.BlancoRestException"</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
     <t>BlancoRestの標準例外クラス名です．</t>
     <phoneticPr fontId="4"/>
   </si>
@@ -602,6 +594,212 @@
   </si>
   <si>
     <t>"0.2.0"</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>HTTP_METHOD_GET</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>"HTTP_METHOD_GET"</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>HTTPメソッドGETを表す文字列</t>
+    <rPh sb="12" eb="13">
+      <t xml:space="preserve">アラワス </t>
+    </rPh>
+    <rPh sb="14" eb="17">
+      <t xml:space="preserve">モジレツ </t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>HTTP_METHOD_POST</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>"HTTP_METHOD_POST"</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>HTTPメソッドPOSTを表す文字列</t>
+    <rPh sb="13" eb="14">
+      <t xml:space="preserve">アラワス </t>
+    </rPh>
+    <rPh sb="15" eb="18">
+      <t xml:space="preserve">モジレツ </t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>HTTP_METHOD_PUT</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>"HTTP_METHOD_PUT"</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>HTTPメソッドPUTを表す文字列</t>
+    <rPh sb="12" eb="13">
+      <t xml:space="preserve">アラワス </t>
+    </rPh>
+    <rPh sb="14" eb="17">
+      <t xml:space="preserve">モジレツ </t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>HTTP_METHOD_DELETE</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>"HTTP_METHOD_DELETE"</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>HTTPメソッドDELETEを表す文字列</t>
+    <rPh sb="15" eb="16">
+      <t xml:space="preserve">アラワス </t>
+    </rPh>
+    <rPh sb="17" eb="20">
+      <t xml:space="preserve">モジレツ </t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>TELEGRAM_INPUT</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>"TELEGRAM_INPUT"</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>電文種別INPUTを表す文字列</t>
+    <rPh sb="0" eb="4">
+      <t xml:space="preserve">デンブンシュベツ </t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t xml:space="preserve">アラワス </t>
+    </rPh>
+    <rPh sb="12" eb="15">
+      <t xml:space="preserve">モジレツ </t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>TELEGRAM_OUTPUT</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>"TELEGRAM_OUTPUT"</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>電文種別OUTPUTを表す文字列</t>
+    <rPh sb="0" eb="4">
+      <t xml:space="preserve">デンブンシュベツ </t>
+    </rPh>
+    <rPh sb="11" eb="12">
+      <t xml:space="preserve">アラワス </t>
+    </rPh>
+    <rPh sb="13" eb="16">
+      <t xml:space="preserve">モジレツ </t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>POST_CONTROLLER_METHOD</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>"doPost"</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>POSTメソッド時に呼ばれるmicronaut controller用メソッド</t>
+    <rPh sb="8" eb="9">
+      <t xml:space="preserve">ジニ </t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t xml:space="preserve">ヨバレル </t>
+    </rPh>
+    <rPh sb="34" eb="35">
+      <t xml:space="preserve">ヨウ </t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>PUT_CONTROLLER_METHOD</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>"doPut"</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>PUTメソッド時に呼ばれるmicronaut controller用メソッド</t>
+    <rPh sb="7" eb="8">
+      <t>ヨ</t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t>ジッコウ</t>
+    </rPh>
+    <rPh sb="17" eb="18">
+      <t>メイ</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>GET_CONTROLLER_METHOD</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>"doGet"</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>GETメソッド時に呼ばれるmicronaut controller用メソッド</t>
+    <rPh sb="7" eb="8">
+      <t>ヨ</t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t>ジッコウ</t>
+    </rPh>
+    <rPh sb="17" eb="18">
+      <t>メイ</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>DELETE_CONTROLLER_METHOD</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>"doDelete"</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>DELETEメソッド時に呼ばれるmicronaut controller用メソッド</t>
+    <rPh sb="10" eb="11">
+      <t>ヨ</t>
+    </rPh>
+    <rPh sb="14" eb="16">
+      <t>ジッコウ</t>
+    </rPh>
+    <rPh sb="20" eb="21">
+      <t>メイ</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>"blanco.restgenerator.common.ApiBase"</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>"blanco.restgenerator.Exception.BlancoRestException"</t>
     <phoneticPr fontId="4"/>
   </si>
 </sst>
@@ -947,7 +1145,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1043,6 +1241,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1483,10 +1684,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H57"/>
+  <dimension ref="A1:H69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1532,7 +1733,7 @@
       </c>
       <c r="B6" s="7"/>
       <c r="C6" s="8" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D6" s="9"/>
       <c r="E6" s="10"/>
@@ -1543,7 +1744,7 @@
       </c>
       <c r="B7" s="7"/>
       <c r="C7" s="11" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D7" s="12"/>
       <c r="E7" s="10"/>
@@ -1554,7 +1755,7 @@
       </c>
       <c r="B8" s="7"/>
       <c r="C8" s="8" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D8" s="13"/>
       <c r="E8" s="13"/>
@@ -1646,19 +1847,19 @@
       <c r="H17"/>
     </row>
     <row r="18" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A18" s="43" t="s">
+      <c r="A18" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="43" t="s">
+      <c r="B18" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="44" t="s">
+      <c r="C18" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="D18" s="44" t="s">
+      <c r="D18" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="E18" s="44" t="s">
+      <c r="E18" s="45" t="s">
         <v>7</v>
       </c>
       <c r="F18" s="22"/>
@@ -1666,11 +1867,11 @@
       <c r="H18"/>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="43"/>
-      <c r="B19" s="43"/>
-      <c r="C19" s="44"/>
-      <c r="D19" s="44"/>
-      <c r="E19" s="44"/>
+      <c r="A19" s="44"/>
+      <c r="B19" s="44"/>
+      <c r="C19" s="45"/>
+      <c r="D19" s="45"/>
+      <c r="E19" s="45"/>
       <c r="F19" s="23"/>
       <c r="G19"/>
       <c r="H19"/>
@@ -1686,7 +1887,7 @@
         <v>22</v>
       </c>
       <c r="D20" s="26" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E20" s="27" t="s">
         <v>23</v>
@@ -1707,7 +1908,7 @@
         <v>22</v>
       </c>
       <c r="D21" s="26" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E21" s="29" t="s">
         <v>25</v>
@@ -1728,7 +1929,7 @@
         <v>22</v>
       </c>
       <c r="D22" s="26" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E22" s="26" t="s">
         <v>27</v>
@@ -1739,7 +1940,7 @@
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="24">
-        <f t="shared" ref="A23:A57" si="0">A22+1</f>
+        <f t="shared" ref="A23:A67" si="0">A22+1</f>
         <v>4</v>
       </c>
       <c r="B23" s="25" t="s">
@@ -1749,7 +1950,7 @@
         <v>22</v>
       </c>
       <c r="D23" s="26" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E23" s="26" t="s">
         <v>29</v>
@@ -1785,16 +1986,16 @@
         <v>6</v>
       </c>
       <c r="B25" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="C25" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="D25" s="26" t="s">
+        <v>109</v>
+      </c>
+      <c r="E25" s="26" t="s">
         <v>110</v>
-      </c>
-      <c r="C25" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="D25" s="26" t="s">
-        <v>111</v>
-      </c>
-      <c r="E25" s="26" t="s">
-        <v>112</v>
       </c>
       <c r="F25" s="30"/>
       <c r="G25"/>
@@ -1806,16 +2007,16 @@
         <v>7</v>
       </c>
       <c r="B26" s="25" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C26" s="26" t="s">
         <v>33</v>
       </c>
       <c r="D26" s="26" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E26" s="26" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F26" s="30"/>
       <c r="G26"/>
@@ -1827,16 +2028,16 @@
         <v>8</v>
       </c>
       <c r="B27" s="25" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C27" s="26" t="s">
         <v>33</v>
       </c>
       <c r="D27" s="26" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E27" s="26" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F27" s="30"/>
       <c r="G27"/>
@@ -1848,16 +2049,16 @@
         <v>9</v>
       </c>
       <c r="B28" s="25" t="s">
+        <v>115</v>
+      </c>
+      <c r="C28" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="D28" s="26" t="s">
+        <v>116</v>
+      </c>
+      <c r="E28" s="26" t="s">
         <v>117</v>
-      </c>
-      <c r="C28" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="D28" s="26" t="s">
-        <v>118</v>
-      </c>
-      <c r="E28" s="26" t="s">
-        <v>119</v>
       </c>
       <c r="F28" s="30"/>
       <c r="G28"/>
@@ -1869,16 +2070,16 @@
         <v>10</v>
       </c>
       <c r="B29" s="25" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C29" s="26" t="s">
         <v>33</v>
       </c>
       <c r="D29" s="26" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E29" s="26" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F29" s="32"/>
       <c r="G29"/>
@@ -1917,7 +2118,7 @@
         <v>33</v>
       </c>
       <c r="D31" s="26" t="s">
-        <v>55</v>
+        <v>151</v>
       </c>
       <c r="E31" s="26" t="s">
         <v>39</v>
@@ -2016,13 +2217,13 @@
         <v>17</v>
       </c>
       <c r="B36" s="25" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C36" s="31" t="s">
         <v>33</v>
       </c>
       <c r="D36" s="31" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E36" s="31" t="s">
         <v>52</v>
@@ -2037,13 +2238,13 @@
         <v>18</v>
       </c>
       <c r="B37" s="25" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C37" s="31" t="s">
         <v>33</v>
       </c>
       <c r="D37" s="31" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E37" s="31" t="s">
         <v>52</v>
@@ -2058,13 +2259,13 @@
         <v>19</v>
       </c>
       <c r="B38" s="25" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C38" s="31" t="s">
         <v>33</v>
       </c>
       <c r="D38" s="31" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E38" s="31" t="s">
         <v>52</v>
@@ -2079,13 +2280,13 @@
         <v>20</v>
       </c>
       <c r="B39" s="25" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C39" s="31" t="s">
         <v>33</v>
       </c>
       <c r="D39" s="31" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E39" s="31" t="s">
         <v>52</v>
@@ -2099,19 +2300,19 @@
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="B40" s="33" t="s">
-        <v>68</v>
-      </c>
-      <c r="C40" s="34" t="s">
-        <v>33</v>
-      </c>
-      <c r="D40" s="34" t="s">
-        <v>60</v>
-      </c>
-      <c r="E40" s="34" t="s">
+      <c r="B40" s="43" t="s">
+        <v>67</v>
+      </c>
+      <c r="C40" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="D40" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="E40" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="F40" s="35"/>
+      <c r="F40" s="30"/>
       <c r="G40"/>
       <c r="H40"/>
     </row>
@@ -2120,19 +2321,19 @@
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="B41" s="33" t="s">
-        <v>69</v>
-      </c>
-      <c r="C41" s="34" t="s">
-        <v>33</v>
-      </c>
-      <c r="D41" s="34" t="s">
-        <v>63</v>
-      </c>
-      <c r="E41" s="34" t="s">
+      <c r="B41" s="43" t="s">
+        <v>68</v>
+      </c>
+      <c r="C41" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="D41" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="E41" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="F41" s="35"/>
+      <c r="F41" s="30"/>
       <c r="G41"/>
       <c r="H41"/>
     </row>
@@ -2141,19 +2342,19 @@
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="B42" s="33" t="s">
-        <v>70</v>
-      </c>
-      <c r="C42" s="34" t="s">
-        <v>33</v>
-      </c>
-      <c r="D42" s="34" t="s">
-        <v>61</v>
-      </c>
-      <c r="E42" s="34" t="s">
+      <c r="B42" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="C42" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="D42" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="E42" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="F42" s="35"/>
+      <c r="F42" s="30"/>
       <c r="G42"/>
       <c r="H42"/>
     </row>
@@ -2162,19 +2363,19 @@
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="B43" s="33" t="s">
-        <v>71</v>
-      </c>
-      <c r="C43" s="34" t="s">
-        <v>33</v>
-      </c>
-      <c r="D43" s="34" t="s">
-        <v>62</v>
-      </c>
-      <c r="E43" s="34" t="s">
+      <c r="B43" s="43" t="s">
+        <v>70</v>
+      </c>
+      <c r="C43" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="D43" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="E43" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="F43" s="35"/>
+      <c r="F43" s="30"/>
       <c r="G43"/>
       <c r="H43"/>
     </row>
@@ -2183,19 +2384,19 @@
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="B44" s="33" t="s">
+      <c r="B44" s="43" t="s">
+        <v>71</v>
+      </c>
+      <c r="C44" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="D44" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="E44" s="26" t="s">
         <v>72</v>
       </c>
-      <c r="C44" s="34" t="s">
-        <v>33</v>
-      </c>
-      <c r="D44" s="34" t="s">
-        <v>108</v>
-      </c>
-      <c r="E44" s="34" t="s">
-        <v>73</v>
-      </c>
-      <c r="F44" s="35"/>
+      <c r="F44" s="30"/>
       <c r="G44"/>
       <c r="H44"/>
     </row>
@@ -2204,19 +2405,19 @@
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="B45" s="33" t="s">
+      <c r="B45" s="43" t="s">
+        <v>73</v>
+      </c>
+      <c r="C45" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="D45" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="E45" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="C45" s="34" t="s">
-        <v>33</v>
-      </c>
-      <c r="D45" s="34" t="s">
-        <v>109</v>
-      </c>
-      <c r="E45" s="34" t="s">
-        <v>75</v>
-      </c>
-      <c r="F45" s="35"/>
+      <c r="F45" s="30"/>
       <c r="G45"/>
       <c r="H45"/>
     </row>
@@ -2225,95 +2426,95 @@
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="B46" s="33" t="s">
-        <v>78</v>
-      </c>
-      <c r="C46" s="34" t="s">
-        <v>33</v>
-      </c>
-      <c r="D46" s="34" t="s">
+      <c r="B46" s="43" t="s">
+        <v>77</v>
+      </c>
+      <c r="C46" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="D46" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="E46" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="E46" s="34" t="s">
-        <v>77</v>
-      </c>
-      <c r="F46" s="35"/>
+      <c r="F46" s="30"/>
     </row>
     <row r="47" spans="1:8">
       <c r="A47" s="24">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="B47" s="33" t="s">
+      <c r="B47" s="43" t="s">
+        <v>78</v>
+      </c>
+      <c r="C47" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="D47" s="26" t="s">
+        <v>152</v>
+      </c>
+      <c r="E47" s="26" t="s">
         <v>79</v>
       </c>
-      <c r="C47" s="34" t="s">
-        <v>33</v>
-      </c>
-      <c r="D47" s="34" t="s">
-        <v>80</v>
-      </c>
-      <c r="E47" s="34" t="s">
-        <v>81</v>
-      </c>
-      <c r="F47" s="35"/>
+      <c r="F47" s="30"/>
     </row>
     <row r="48" spans="1:8">
       <c r="A48" s="24">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="B48" s="33" t="s">
-        <v>84</v>
-      </c>
-      <c r="C48" s="34" t="s">
-        <v>33</v>
-      </c>
-      <c r="D48" s="34" t="s">
-        <v>101</v>
-      </c>
-      <c r="E48" s="34" t="s">
+      <c r="B48" s="43" t="s">
         <v>82</v>
       </c>
-      <c r="F48" s="35"/>
+      <c r="C48" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="D48" s="26" t="s">
+        <v>99</v>
+      </c>
+      <c r="E48" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="F48" s="30"/>
     </row>
     <row r="49" spans="1:8">
       <c r="A49" s="24">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="B49" s="33" t="s">
+      <c r="B49" s="43" t="s">
+        <v>81</v>
+      </c>
+      <c r="C49" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="D49" s="26" t="s">
         <v>83</v>
       </c>
-      <c r="C49" s="34" t="s">
-        <v>33</v>
-      </c>
-      <c r="D49" s="34" t="s">
-        <v>85</v>
-      </c>
-      <c r="E49" s="34" t="s">
-        <v>86</v>
-      </c>
-      <c r="F49" s="35"/>
+      <c r="E49" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="F49" s="30"/>
     </row>
     <row r="50" spans="1:8">
       <c r="A50" s="24">
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="B50" s="25" t="s">
-        <v>87</v>
-      </c>
-      <c r="C50" s="31" t="s">
-        <v>33</v>
-      </c>
-      <c r="D50" s="31" t="s">
-        <v>95</v>
-      </c>
-      <c r="E50" s="31" t="s">
-        <v>100</v>
-      </c>
-      <c r="F50" s="32"/>
+      <c r="B50" s="43" t="s">
+        <v>85</v>
+      </c>
+      <c r="C50" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="D50" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="E50" s="26" t="s">
+        <v>98</v>
+      </c>
+      <c r="F50" s="30"/>
       <c r="G50"/>
       <c r="H50"/>
     </row>
@@ -2322,19 +2523,19 @@
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="B51" s="25" t="s">
-        <v>88</v>
-      </c>
-      <c r="C51" s="31" t="s">
-        <v>33</v>
-      </c>
-      <c r="D51" s="31" t="s">
-        <v>96</v>
-      </c>
-      <c r="E51" s="31" t="s">
-        <v>99</v>
-      </c>
-      <c r="F51" s="32"/>
+      <c r="B51" s="43" t="s">
+        <v>86</v>
+      </c>
+      <c r="C51" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="D51" s="26" t="s">
+        <v>94</v>
+      </c>
+      <c r="E51" s="26" t="s">
+        <v>97</v>
+      </c>
+      <c r="F51" s="30"/>
       <c r="G51"/>
       <c r="H51"/>
     </row>
@@ -2343,19 +2544,19 @@
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
-      <c r="B52" s="25" t="s">
-        <v>89</v>
-      </c>
-      <c r="C52" s="31" t="s">
-        <v>33</v>
-      </c>
-      <c r="D52" s="31" t="s">
+      <c r="B52" s="43" t="s">
+        <v>87</v>
+      </c>
+      <c r="C52" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="D52" s="26" t="s">
+        <v>95</v>
+      </c>
+      <c r="E52" s="26" t="s">
         <v>97</v>
       </c>
-      <c r="E52" s="31" t="s">
-        <v>99</v>
-      </c>
-      <c r="F52" s="32"/>
+      <c r="F52" s="30"/>
       <c r="G52"/>
       <c r="H52"/>
     </row>
@@ -2364,19 +2565,19 @@
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
-      <c r="B53" s="25" t="s">
-        <v>90</v>
-      </c>
-      <c r="C53" s="31" t="s">
-        <v>33</v>
-      </c>
-      <c r="D53" s="31" t="s">
-        <v>98</v>
-      </c>
-      <c r="E53" s="31" t="s">
-        <v>99</v>
-      </c>
-      <c r="F53" s="32"/>
+      <c r="B53" s="43" t="s">
+        <v>88</v>
+      </c>
+      <c r="C53" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="D53" s="26" t="s">
+        <v>96</v>
+      </c>
+      <c r="E53" s="26" t="s">
+        <v>97</v>
+      </c>
+      <c r="F53" s="30"/>
       <c r="G53"/>
       <c r="H53"/>
     </row>
@@ -2385,19 +2586,19 @@
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
-      <c r="B54" s="33" t="s">
-        <v>91</v>
-      </c>
-      <c r="C54" s="34" t="s">
-        <v>33</v>
-      </c>
-      <c r="D54" s="34" t="s">
-        <v>95</v>
-      </c>
-      <c r="E54" s="34" t="s">
-        <v>99</v>
-      </c>
-      <c r="F54" s="35"/>
+      <c r="B54" s="43" t="s">
+        <v>89</v>
+      </c>
+      <c r="C54" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="D54" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="E54" s="26" t="s">
+        <v>97</v>
+      </c>
+      <c r="F54" s="30"/>
       <c r="G54"/>
       <c r="H54"/>
     </row>
@@ -2406,19 +2607,19 @@
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
-      <c r="B55" s="33" t="s">
-        <v>92</v>
-      </c>
-      <c r="C55" s="34" t="s">
-        <v>33</v>
-      </c>
-      <c r="D55" s="34" t="s">
-        <v>96</v>
-      </c>
-      <c r="E55" s="34" t="s">
-        <v>99</v>
-      </c>
-      <c r="F55" s="35"/>
+      <c r="B55" s="43" t="s">
+        <v>90</v>
+      </c>
+      <c r="C55" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="D55" s="26" t="s">
+        <v>94</v>
+      </c>
+      <c r="E55" s="26" t="s">
+        <v>97</v>
+      </c>
+      <c r="F55" s="30"/>
       <c r="G55"/>
       <c r="H55"/>
     </row>
@@ -2427,19 +2628,19 @@
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="B56" s="33" t="s">
-        <v>93</v>
-      </c>
-      <c r="C56" s="34" t="s">
-        <v>33</v>
-      </c>
-      <c r="D56" s="34" t="s">
+      <c r="B56" s="43" t="s">
+        <v>91</v>
+      </c>
+      <c r="C56" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="D56" s="26" t="s">
+        <v>95</v>
+      </c>
+      <c r="E56" s="26" t="s">
         <v>97</v>
       </c>
-      <c r="E56" s="34" t="s">
-        <v>99</v>
-      </c>
-      <c r="F56" s="35"/>
+      <c r="F56" s="30"/>
       <c r="G56"/>
       <c r="H56"/>
     </row>
@@ -2448,21 +2649,251 @@
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
-      <c r="B57" s="33" t="s">
-        <v>94</v>
-      </c>
-      <c r="C57" s="34" t="s">
-        <v>33</v>
-      </c>
-      <c r="D57" s="34" t="s">
-        <v>98</v>
-      </c>
-      <c r="E57" s="34" t="s">
-        <v>99</v>
-      </c>
-      <c r="F57" s="35"/>
+      <c r="B57" s="43" t="s">
+        <v>92</v>
+      </c>
+      <c r="C57" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="D57" s="26" t="s">
+        <v>96</v>
+      </c>
+      <c r="E57" s="26" t="s">
+        <v>97</v>
+      </c>
+      <c r="F57" s="30"/>
       <c r="G57"/>
       <c r="H57"/>
+    </row>
+    <row r="58" spans="1:8" s="42" customFormat="1">
+      <c r="A58" s="24">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="B58" s="43" t="s">
+        <v>121</v>
+      </c>
+      <c r="C58" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="D58" s="26" t="s">
+        <v>122</v>
+      </c>
+      <c r="E58" s="26" t="s">
+        <v>123</v>
+      </c>
+      <c r="F58" s="30"/>
+      <c r="G58"/>
+      <c r="H58"/>
+    </row>
+    <row r="59" spans="1:8" s="42" customFormat="1">
+      <c r="A59" s="24">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="B59" s="43" t="s">
+        <v>124</v>
+      </c>
+      <c r="C59" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="D59" s="26" t="s">
+        <v>125</v>
+      </c>
+      <c r="E59" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="F59" s="30"/>
+      <c r="G59"/>
+      <c r="H59"/>
+    </row>
+    <row r="60" spans="1:8" s="42" customFormat="1">
+      <c r="A60" s="24">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="B60" s="43" t="s">
+        <v>127</v>
+      </c>
+      <c r="C60" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="D60" s="26" t="s">
+        <v>128</v>
+      </c>
+      <c r="E60" s="26" t="s">
+        <v>129</v>
+      </c>
+      <c r="F60" s="30"/>
+      <c r="G60"/>
+      <c r="H60"/>
+    </row>
+    <row r="61" spans="1:8" s="42" customFormat="1">
+      <c r="A61" s="24">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="B61" s="43" t="s">
+        <v>130</v>
+      </c>
+      <c r="C61" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="D61" s="26" t="s">
+        <v>131</v>
+      </c>
+      <c r="E61" s="26" t="s">
+        <v>132</v>
+      </c>
+      <c r="F61" s="30"/>
+      <c r="G61"/>
+      <c r="H61"/>
+    </row>
+    <row r="62" spans="1:8" s="42" customFormat="1">
+      <c r="A62" s="24">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="B62" s="43" t="s">
+        <v>133</v>
+      </c>
+      <c r="C62" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="D62" s="26" t="s">
+        <v>134</v>
+      </c>
+      <c r="E62" s="26" t="s">
+        <v>135</v>
+      </c>
+      <c r="F62" s="30"/>
+      <c r="G62"/>
+      <c r="H62"/>
+    </row>
+    <row r="63" spans="1:8" s="42" customFormat="1">
+      <c r="A63" s="24">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="B63" s="43" t="s">
+        <v>136</v>
+      </c>
+      <c r="C63" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="D63" s="26" t="s">
+        <v>137</v>
+      </c>
+      <c r="E63" s="26" t="s">
+        <v>138</v>
+      </c>
+      <c r="F63" s="30"/>
+      <c r="G63"/>
+      <c r="H63"/>
+    </row>
+    <row r="64" spans="1:8" s="42" customFormat="1">
+      <c r="A64" s="24">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="B64" s="43" t="s">
+        <v>139</v>
+      </c>
+      <c r="C64" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="D64" s="26" t="s">
+        <v>140</v>
+      </c>
+      <c r="E64" s="26" t="s">
+        <v>141</v>
+      </c>
+      <c r="F64" s="30"/>
+      <c r="G64"/>
+      <c r="H64"/>
+    </row>
+    <row r="65" spans="1:8" s="42" customFormat="1">
+      <c r="A65" s="24">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="B65" s="43" t="s">
+        <v>142</v>
+      </c>
+      <c r="C65" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="D65" s="26" t="s">
+        <v>143</v>
+      </c>
+      <c r="E65" s="26" t="s">
+        <v>144</v>
+      </c>
+      <c r="F65" s="30"/>
+      <c r="G65"/>
+      <c r="H65"/>
+    </row>
+    <row r="66" spans="1:8" s="42" customFormat="1">
+      <c r="A66" s="24">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="B66" s="43" t="s">
+        <v>145</v>
+      </c>
+      <c r="C66" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="D66" s="26" t="s">
+        <v>146</v>
+      </c>
+      <c r="E66" s="26" t="s">
+        <v>147</v>
+      </c>
+      <c r="F66" s="30"/>
+      <c r="G66"/>
+      <c r="H66"/>
+    </row>
+    <row r="67" spans="1:8" s="42" customFormat="1">
+      <c r="A67" s="24">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="B67" s="43" t="s">
+        <v>148</v>
+      </c>
+      <c r="C67" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="D67" s="26" t="s">
+        <v>149</v>
+      </c>
+      <c r="E67" s="26" t="s">
+        <v>150</v>
+      </c>
+      <c r="F67" s="30"/>
+      <c r="G67"/>
+      <c r="H67"/>
+    </row>
+    <row r="68" spans="1:8" s="42" customFormat="1">
+      <c r="A68" s="24"/>
+      <c r="B68" s="43"/>
+      <c r="C68" s="26"/>
+      <c r="D68" s="26"/>
+      <c r="E68" s="26"/>
+      <c r="F68" s="30"/>
+      <c r="G68"/>
+      <c r="H68"/>
+    </row>
+    <row r="69" spans="1:8" s="42" customFormat="1">
+      <c r="A69" s="24"/>
+      <c r="B69" s="33"/>
+      <c r="C69" s="34"/>
+      <c r="D69" s="34"/>
+      <c r="E69" s="34"/>
+      <c r="F69" s="35"/>
+      <c r="G69"/>
+      <c r="H69"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -2474,7 +2905,7 @@
   </mergeCells>
   <phoneticPr fontId="4"/>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D58" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D70" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>型</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
just for recording: full refactoring for sharing kotlin definition sheets.
</commit_message>
<xml_diff>
--- a/meta/program/BlancoRestGeneratorConstants.xlsx
+++ b/meta/program/BlancoRestGeneratorConstants.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoRestGenerator/meta/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41A4EADB-58DB-5344-9CCD-5FA326823284}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CCA7F0E-0FFC-5348-8FCC-7420C8A84242}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1460" yWindow="1700" windowWidth="22700" windowHeight="15280" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1686,7 +1686,7 @@
   </sheetPr>
   <dimension ref="A1:H69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
       <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
0.2.1: Improvement for default exception generation.
</commit_message>
<xml_diff>
--- a/meta/program/BlancoRestGeneratorConstants.xlsx
+++ b/meta/program/BlancoRestGeneratorConstants.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoRestGenerator/meta/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CCA7F0E-0FFC-5348-8FCC-7420C8A84242}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{374C43CD-E286-4147-9752-22A96E0196FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1460" yWindow="1700" windowWidth="22700" windowHeight="15280" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2100" yWindow="1840" windowWidth="22700" windowHeight="15280" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="constants" sheetId="1" r:id="rId1"/>
@@ -799,7 +799,7 @@
     <phoneticPr fontId="4"/>
   </si>
   <si>
-    <t>"blanco.restgenerator.Exception.BlancoRestException"</t>
+    <t>"blanco.restgenerator.exception.BlancoRestException"</t>
     <phoneticPr fontId="4"/>
   </si>
 </sst>
@@ -1687,7 +1687,7 @@
   <dimension ref="A1:H69"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="D49" sqref="D49"/>
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>

</xml_diff>